<commit_message>
update results of model performance in new runs
</commit_message>
<xml_diff>
--- a/model_performance_summary.xlsx
+++ b/model_performance_summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10102"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kai/Desktop/Article 6/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kai/Desktop/Article_6/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8EE9E55-B57B-F042-90BF-5FF2FC59A630}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8586D1FE-2DA3-5044-9FBC-1515454A26F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4060" yWindow="5240" windowWidth="28040" windowHeight="16700" xr2:uid="{4B26C0E9-1936-1440-92E7-3F4E3D197B1B}"/>
+    <workbookView xWindow="8320" yWindow="9520" windowWidth="28040" windowHeight="16700" xr2:uid="{4B26C0E9-1936-1440-92E7-3F4E3D197B1B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -428,7 +428,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F9"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -491,10 +491,10 @@
         <v>0.74</v>
       </c>
       <c r="E3" s="1">
-        <v>10129</v>
+        <v>9754</v>
       </c>
       <c r="F3" s="1">
-        <v>11135</v>
+        <v>10794</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -505,16 +505,16 @@
         <v>9</v>
       </c>
       <c r="C4" s="1">
-        <v>0.66</v>
+        <v>0.69</v>
       </c>
       <c r="D4" s="1">
-        <v>0.65</v>
+        <v>0.67</v>
       </c>
       <c r="E4" s="1">
-        <v>14325</v>
+        <v>13663.7</v>
       </c>
       <c r="F4" s="1">
-        <v>15165</v>
+        <v>14000</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -525,16 +525,16 @@
         <v>10</v>
       </c>
       <c r="C5" s="1">
-        <v>0.73</v>
+        <v>0.77</v>
       </c>
       <c r="D5" s="1">
-        <v>0.73</v>
+        <v>0.75</v>
       </c>
       <c r="E5" s="1">
-        <v>11100</v>
+        <v>10206</v>
       </c>
       <c r="F5" s="1">
-        <v>11689</v>
+        <v>10689</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -545,16 +545,16 @@
         <v>8</v>
       </c>
       <c r="C6" s="1">
-        <v>0.77</v>
+        <v>0.76</v>
       </c>
       <c r="D6" s="1">
         <v>0.74</v>
       </c>
       <c r="E6" s="1">
-        <v>10520</v>
+        <v>10608</v>
       </c>
       <c r="F6" s="1">
-        <v>11330</v>
+        <v>11434.8</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -571,10 +571,10 @@
         <v>0.82</v>
       </c>
       <c r="E7" s="1">
-        <v>7129</v>
+        <v>7121</v>
       </c>
       <c r="F7" s="1">
-        <v>7634</v>
+        <v>7741</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -591,10 +591,10 @@
         <v>0.73</v>
       </c>
       <c r="E8" s="1">
-        <v>11570</v>
+        <v>11439</v>
       </c>
       <c r="F8" s="1">
-        <v>11320</v>
+        <v>11312</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -605,16 +605,16 @@
         <v>10</v>
       </c>
       <c r="C9" s="1">
-        <v>0.82</v>
+        <v>0.81</v>
       </c>
       <c r="D9" s="1">
         <v>0.82</v>
       </c>
       <c r="E9" s="1">
-        <v>7575</v>
+        <v>7816</v>
       </c>
       <c r="F9" s="1">
-        <v>7866</v>
+        <v>7988</v>
       </c>
     </row>
   </sheetData>

</xml_diff>